<commit_message>
Add initial database entries for car models and sales ratings; implement sentiment analysis notebook
- Created a new JavaScript file to insert car data into the database, including details like brand, model, price, fuel consumption, and power specifications.
- Added a collection for sales ratings with associated safety ratings and projected sales for 2024.
- Developed a Jupyter notebook for sentiment analysis using Naive Bayes, including text preprocessing, model training, and evaluation.
- Integrated Sastrawi library for Indonesian text processing, including stopword removal and stemming.
- Implemented functionality to analyze user input for sentiment predictions.
</commit_message>
<xml_diff>
--- a/tgs3/Hasil prediksi SVM.xlsx
+++ b/tgs3/Hasil prediksi SVM.xlsx
@@ -442,202 +442,202 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>